<commit_message>
free bonus edit ...
</commit_message>
<xml_diff>
--- a/features/backlog/android/app_crushing_report_settings.xlsx
+++ b/features/backlog/android/app_crushing_report_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4D7D44-1412-4A6A-A659-F86825DB1DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C905E3-388C-4F78-B6B5-D15549896BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -153,190 +153,35 @@
     <t>Test case scenario : App Crushing Report</t>
   </si>
   <si>
-    <t>Test the notification toggle with different language settings to ensure proper localization.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle on Android emulators with different configurations.</t>
-  </si>
-  <si>
-    <t>Toggle notifications in different display modes, such as night mode or dark mode.</t>
-  </si>
-  <si>
-    <t>Uninstall and reinstall the app. Verify that the notification toggle state is reset to the default.</t>
-  </si>
-  <si>
-    <t>Toggle notifications and then revoke app permissions to confirm the expected behavior.</t>
-  </si>
-  <si>
-    <t>Toggle notifications while the device is in silent mode. Confirm that the app respects the device's silent mode settings.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle while the app has background processes running.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle in different time zones to ensure proper functionality.</t>
-  </si>
-  <si>
-    <t>Verify that the notification toggle accommodates accessibility settings.</t>
-  </si>
-  <si>
-    <t>Assess the app's responsiveness when the notification toggle is used during heavy app usage.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle when the app interacts with other apps on the device.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle in both portrait and landscape orientations.</t>
-  </si>
-  <si>
-    <t>Confirm that the notification toggle works seamlessly with apps configured in different languages.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle on older versions of the app to ensure backward compatibility.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle while the app is stored on external storage.</t>
-  </si>
-  <si>
-    <t>Toggle notifications when the device is in low battery mode.</t>
-  </si>
-  <si>
-    <t>Confirm that the app provides in-app notifications based on the toggle state.</t>
-  </si>
-  <si>
-    <t>Toggle notifications while connected to Bluetooth devices.</t>
-  </si>
-  <si>
-    <t>Verify that enabling notifications prompts the user with the appropriate permissions dialog.</t>
-  </si>
-  <si>
-    <t>Confirm that the app allows users to customize notification preferences.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle on devices with different screen resolutions.</t>
-  </si>
-  <si>
-    <t>Toggle notifications during the app initialization process.</t>
-  </si>
-  <si>
-    <t>Verify that the notification toggle does not interfere with essential background tasks.</t>
-  </si>
-  <si>
-    <t>Test different priority levels for notifications.</t>
-  </si>
-  <si>
-    <t>Confirm that the notification toggle adheres to Android's accessibility features.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle when the app is subject to Android's background limitations.</t>
-  </si>
-  <si>
-    <t>Toggle notifications and then reset app permissions. Confirm the expected behavior.</t>
-  </si>
-  <si>
-    <t>Test the notification toggle in an app that integrates third-party libraries for notification services.</t>
-  </si>
-  <si>
-    <t>Confirm that the app handles silent notifications appropriately.</t>
-  </si>
-  <si>
-    <t>Verify that enabling notifications does not require additional auto</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-016</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-017</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-018</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-019</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-020</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-021</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-022</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-023</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-024</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-025</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-026</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-027</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-028</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-029</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-030</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-031</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-032</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-033</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-034</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-035</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-036</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-037</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-038</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-039</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-040</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-041</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-042</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-043</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-044</t>
-  </si>
-  <si>
-    <t>SYMAPPCRUS-045</t>
+    <t>1. Open the app
+2. travers the app
+3. check and find any crushing point
+4. analyze the app crushing data.</t>
   </si>
   <si>
     <t>1. Open the app
 2. travers the app
 3. check and find any crushing point
-4. analyze the app crushing data.</t>
+4. observe the slow after app crusing.</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. travers the app
+3. check and find any crushing point
+4. differentiate the app crusing messge for multiple crush.</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. travers the app
+3. check and find any crushing point
+4. make sure app is running on os 17.</t>
+  </si>
+  <si>
+    <t>1. Open the app
+2. travers the app
+3. check and find any crushing point
+4. open the reporting tools
+5. observe the data.</t>
   </si>
 </sst>
 </file>
@@ -391,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -414,24 +259,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -461,9 +293,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1140,7 +969,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G48" headerRowDxfId="8" totalsRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G18" headerRowDxfId="8" totalsRowDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1358,8 +1187,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1376,15 +1205,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1406,13 +1235,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1528,7 +1357,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>8</v>
@@ -1566,7 +1395,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>8</v>
@@ -1593,7 +1422,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1604,7 +1433,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>8</v>
@@ -1642,7 +1471,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>8</v>
@@ -1680,7 +1509,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>8</v>
@@ -1718,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>8</v>
@@ -1756,7 +1585,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>8</v>
@@ -1783,7 +1612,7 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -1794,7 +1623,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>8</v>
@@ -1821,7 +1650,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
@@ -1832,7 +1661,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>8</v>
@@ -1859,7 +1688,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
@@ -1870,7 +1699,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>8</v>
@@ -1897,7 +1726,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
@@ -1908,7 +1737,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>8</v>
@@ -1935,7 +1764,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
@@ -1946,7 +1775,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>8</v>
@@ -1984,7 +1813,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>8</v>
@@ -2011,7 +1840,7 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
@@ -2050,23 +1879,13 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="12"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2088,23 +1907,13 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="12"/>
+      <c r="G20" s="10"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2126,23 +1935,13 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="12"/>
+      <c r="G21" s="10"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2164,23 +1963,13 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="12"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2202,23 +1991,13 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="12"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2240,23 +2019,13 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="12"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2278,23 +2047,13 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="12"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2316,23 +2075,13 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="12"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2354,23 +2103,13 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="12"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2392,23 +2131,13 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="12"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2430,23 +2159,13 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="12"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2468,23 +2187,13 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="10"/>
-      <c r="G30" s="12"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -2506,23 +2215,13 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="12"/>
+      <c r="G31" s="10"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -2544,23 +2243,13 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="10"/>
-      <c r="G32" s="12"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2582,23 +2271,13 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="12"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -2620,23 +2299,13 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="10"/>
-      <c r="G34" s="12"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -2658,23 +2327,13 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
       <c r="F35" s="10"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2696,23 +2355,13 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2734,23 +2383,13 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="10"/>
-      <c r="G37" s="12"/>
+      <c r="G37" s="10"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2772,23 +2411,13 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="10"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2810,23 +2439,13 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
       <c r="F39" s="10"/>
-      <c r="G39" s="12"/>
+      <c r="G39" s="10"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2848,23 +2467,13 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="12"/>
+      <c r="G40" s="10"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2886,23 +2495,13 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="12"/>
+      <c r="G41" s="10"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2924,23 +2523,13 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="12"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2962,23 +2551,13 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="12"/>
+      <c r="G43" s="10"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -3000,23 +2579,13 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="12"/>
+      <c r="G44" s="10"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -3038,23 +2607,13 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
       <c r="F45" s="10"/>
-      <c r="G45" s="12"/>
+      <c r="G45" s="10"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -3076,23 +2635,13 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
       <c r="F46" s="10"/>
-      <c r="G46" s="12"/>
+      <c r="G46" s="10"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -3114,23 +2663,13 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="12"/>
+      <c r="G47" s="10"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -3152,23 +2691,13 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="10"/>
-      <c r="G48" s="12"/>
+      <c r="G48" s="10"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -28725,14 +28254,7 @@
       <c r="Y960" s="1"/>
       <c r="Z960" s="1"/>
     </row>
-    <row r="961" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A961" s="10"/>
-      <c r="B961" s="10"/>
-      <c r="C961" s="8"/>
-      <c r="D961" s="10"/>
-      <c r="E961" s="10"/>
-      <c r="F961" s="10"/>
-      <c r="G961" s="10"/>
+    <row r="961" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H961" s="1"/>
       <c r="I961" s="1"/>
       <c r="J961" s="1"/>
@@ -28753,14 +28275,7 @@
       <c r="Y961" s="1"/>
       <c r="Z961" s="1"/>
     </row>
-    <row r="962" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A962" s="10"/>
-      <c r="B962" s="10"/>
-      <c r="C962" s="8"/>
-      <c r="D962" s="10"/>
-      <c r="E962" s="10"/>
-      <c r="F962" s="10"/>
-      <c r="G962" s="10"/>
+    <row r="962" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H962" s="1"/>
       <c r="I962" s="1"/>
       <c r="J962" s="1"/>
@@ -28781,14 +28296,7 @@
       <c r="Y962" s="1"/>
       <c r="Z962" s="1"/>
     </row>
-    <row r="963" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A963" s="10"/>
-      <c r="B963" s="10"/>
-      <c r="C963" s="8"/>
-      <c r="D963" s="10"/>
-      <c r="E963" s="10"/>
-      <c r="F963" s="10"/>
-      <c r="G963" s="10"/>
+    <row r="963" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H963" s="1"/>
       <c r="I963" s="1"/>
       <c r="J963" s="1"/>
@@ -28809,14 +28317,7 @@
       <c r="Y963" s="1"/>
       <c r="Z963" s="1"/>
     </row>
-    <row r="964" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A964" s="10"/>
-      <c r="B964" s="10"/>
-      <c r="C964" s="8"/>
-      <c r="D964" s="10"/>
-      <c r="E964" s="10"/>
-      <c r="F964" s="10"/>
-      <c r="G964" s="10"/>
+    <row r="964" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H964" s="1"/>
       <c r="I964" s="1"/>
       <c r="J964" s="1"/>
@@ -28837,14 +28338,7 @@
       <c r="Y964" s="1"/>
       <c r="Z964" s="1"/>
     </row>
-    <row r="965" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A965" s="10"/>
-      <c r="B965" s="10"/>
-      <c r="C965" s="8"/>
-      <c r="D965" s="10"/>
-      <c r="E965" s="10"/>
-      <c r="F965" s="10"/>
-      <c r="G965" s="10"/>
+    <row r="965" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H965" s="1"/>
       <c r="I965" s="1"/>
       <c r="J965" s="1"/>
@@ -28865,14 +28359,7 @@
       <c r="Y965" s="1"/>
       <c r="Z965" s="1"/>
     </row>
-    <row r="966" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A966" s="10"/>
-      <c r="B966" s="10"/>
-      <c r="C966" s="8"/>
-      <c r="D966" s="10"/>
-      <c r="E966" s="10"/>
-      <c r="F966" s="10"/>
-      <c r="G966" s="10"/>
+    <row r="966" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H966" s="1"/>
       <c r="I966" s="1"/>
       <c r="J966" s="1"/>
@@ -28893,14 +28380,7 @@
       <c r="Y966" s="1"/>
       <c r="Z966" s="1"/>
     </row>
-    <row r="967" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A967" s="10"/>
-      <c r="B967" s="10"/>
-      <c r="C967" s="8"/>
-      <c r="D967" s="10"/>
-      <c r="E967" s="10"/>
-      <c r="F967" s="10"/>
-      <c r="G967" s="10"/>
+    <row r="967" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H967" s="1"/>
       <c r="I967" s="1"/>
       <c r="J967" s="1"/>
@@ -28921,14 +28401,7 @@
       <c r="Y967" s="1"/>
       <c r="Z967" s="1"/>
     </row>
-    <row r="968" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A968" s="10"/>
-      <c r="B968" s="10"/>
-      <c r="C968" s="8"/>
-      <c r="D968" s="10"/>
-      <c r="E968" s="10"/>
-      <c r="F968" s="10"/>
-      <c r="G968" s="10"/>
+    <row r="968" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H968" s="1"/>
       <c r="I968" s="1"/>
       <c r="J968" s="1"/>
@@ -28949,14 +28422,7 @@
       <c r="Y968" s="1"/>
       <c r="Z968" s="1"/>
     </row>
-    <row r="969" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A969" s="10"/>
-      <c r="B969" s="10"/>
-      <c r="C969" s="8"/>
-      <c r="D969" s="10"/>
-      <c r="E969" s="10"/>
-      <c r="F969" s="10"/>
-      <c r="G969" s="10"/>
+    <row r="969" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H969" s="1"/>
       <c r="I969" s="1"/>
       <c r="J969" s="1"/>
@@ -28977,14 +28443,7 @@
       <c r="Y969" s="1"/>
       <c r="Z969" s="1"/>
     </row>
-    <row r="970" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A970" s="10"/>
-      <c r="B970" s="10"/>
-      <c r="C970" s="8"/>
-      <c r="D970" s="10"/>
-      <c r="E970" s="10"/>
-      <c r="F970" s="10"/>
-      <c r="G970" s="10"/>
+    <row r="970" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H970" s="1"/>
       <c r="I970" s="1"/>
       <c r="J970" s="1"/>
@@ -29005,14 +28464,7 @@
       <c r="Y970" s="1"/>
       <c r="Z970" s="1"/>
     </row>
-    <row r="971" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A971" s="10"/>
-      <c r="B971" s="10"/>
-      <c r="C971" s="8"/>
-      <c r="D971" s="10"/>
-      <c r="E971" s="10"/>
-      <c r="F971" s="10"/>
-      <c r="G971" s="10"/>
+    <row r="971" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H971" s="1"/>
       <c r="I971" s="1"/>
       <c r="J971" s="1"/>
@@ -29033,14 +28485,7 @@
       <c r="Y971" s="1"/>
       <c r="Z971" s="1"/>
     </row>
-    <row r="972" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A972" s="10"/>
-      <c r="B972" s="10"/>
-      <c r="C972" s="8"/>
-      <c r="D972" s="10"/>
-      <c r="E972" s="10"/>
-      <c r="F972" s="10"/>
-      <c r="G972" s="10"/>
+    <row r="972" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H972" s="1"/>
       <c r="I972" s="1"/>
       <c r="J972" s="1"/>
@@ -29061,14 +28506,7 @@
       <c r="Y972" s="1"/>
       <c r="Z972" s="1"/>
     </row>
-    <row r="973" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A973" s="10"/>
-      <c r="B973" s="10"/>
-      <c r="C973" s="8"/>
-      <c r="D973" s="10"/>
-      <c r="E973" s="10"/>
-      <c r="F973" s="10"/>
-      <c r="G973" s="10"/>
+    <row r="973" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H973" s="1"/>
       <c r="I973" s="1"/>
       <c r="J973" s="1"/>
@@ -29089,14 +28527,7 @@
       <c r="Y973" s="1"/>
       <c r="Z973" s="1"/>
     </row>
-    <row r="974" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A974" s="10"/>
-      <c r="B974" s="10"/>
-      <c r="C974" s="8"/>
-      <c r="D974" s="10"/>
-      <c r="E974" s="10"/>
-      <c r="F974" s="10"/>
-      <c r="G974" s="10"/>
+    <row r="974" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H974" s="1"/>
       <c r="I974" s="1"/>
       <c r="J974" s="1"/>
@@ -29117,14 +28548,7 @@
       <c r="Y974" s="1"/>
       <c r="Z974" s="1"/>
     </row>
-    <row r="975" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A975" s="10"/>
-      <c r="B975" s="10"/>
-      <c r="C975" s="8"/>
-      <c r="D975" s="10"/>
-      <c r="E975" s="10"/>
-      <c r="F975" s="10"/>
-      <c r="G975" s="10"/>
+    <row r="975" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H975" s="1"/>
       <c r="I975" s="1"/>
       <c r="J975" s="1"/>
@@ -29145,14 +28569,7 @@
       <c r="Y975" s="1"/>
       <c r="Z975" s="1"/>
     </row>
-    <row r="976" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A976" s="10"/>
-      <c r="B976" s="10"/>
-      <c r="C976" s="8"/>
-      <c r="D976" s="10"/>
-      <c r="E976" s="10"/>
-      <c r="F976" s="10"/>
-      <c r="G976" s="10"/>
+    <row r="976" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H976" s="1"/>
       <c r="I976" s="1"/>
       <c r="J976" s="1"/>
@@ -29173,14 +28590,7 @@
       <c r="Y976" s="1"/>
       <c r="Z976" s="1"/>
     </row>
-    <row r="977" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A977" s="10"/>
-      <c r="B977" s="10"/>
-      <c r="C977" s="8"/>
-      <c r="D977" s="10"/>
-      <c r="E977" s="10"/>
-      <c r="F977" s="10"/>
-      <c r="G977" s="10"/>
+    <row r="977" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H977" s="1"/>
       <c r="I977" s="1"/>
       <c r="J977" s="1"/>
@@ -29201,14 +28611,7 @@
       <c r="Y977" s="1"/>
       <c r="Z977" s="1"/>
     </row>
-    <row r="978" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A978" s="10"/>
-      <c r="B978" s="10"/>
-      <c r="C978" s="8"/>
-      <c r="D978" s="10"/>
-      <c r="E978" s="10"/>
-      <c r="F978" s="10"/>
-      <c r="G978" s="10"/>
+    <row r="978" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H978" s="1"/>
       <c r="I978" s="1"/>
       <c r="J978" s="1"/>
@@ -29229,14 +28632,7 @@
       <c r="Y978" s="1"/>
       <c r="Z978" s="1"/>
     </row>
-    <row r="979" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A979" s="10"/>
-      <c r="B979" s="10"/>
-      <c r="C979" s="8"/>
-      <c r="D979" s="10"/>
-      <c r="E979" s="10"/>
-      <c r="F979" s="10"/>
-      <c r="G979" s="10"/>
+    <row r="979" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H979" s="1"/>
       <c r="I979" s="1"/>
       <c r="J979" s="1"/>
@@ -29257,14 +28653,7 @@
       <c r="Y979" s="1"/>
       <c r="Z979" s="1"/>
     </row>
-    <row r="980" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A980" s="10"/>
-      <c r="B980" s="10"/>
-      <c r="C980" s="8"/>
-      <c r="D980" s="10"/>
-      <c r="E980" s="10"/>
-      <c r="F980" s="10"/>
-      <c r="G980" s="10"/>
+    <row r="980" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H980" s="1"/>
       <c r="I980" s="1"/>
       <c r="J980" s="1"/>
@@ -29285,14 +28674,7 @@
       <c r="Y980" s="1"/>
       <c r="Z980" s="1"/>
     </row>
-    <row r="981" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A981" s="10"/>
-      <c r="B981" s="10"/>
-      <c r="C981" s="8"/>
-      <c r="D981" s="10"/>
-      <c r="E981" s="10"/>
-      <c r="F981" s="10"/>
-      <c r="G981" s="10"/>
+    <row r="981" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H981" s="1"/>
       <c r="I981" s="1"/>
       <c r="J981" s="1"/>
@@ -29313,14 +28695,7 @@
       <c r="Y981" s="1"/>
       <c r="Z981" s="1"/>
     </row>
-    <row r="982" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A982" s="10"/>
-      <c r="B982" s="10"/>
-      <c r="C982" s="8"/>
-      <c r="D982" s="10"/>
-      <c r="E982" s="10"/>
-      <c r="F982" s="10"/>
-      <c r="G982" s="10"/>
+    <row r="982" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H982" s="1"/>
       <c r="I982" s="1"/>
       <c r="J982" s="1"/>
@@ -29341,14 +28716,7 @@
       <c r="Y982" s="1"/>
       <c r="Z982" s="1"/>
     </row>
-    <row r="983" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A983" s="10"/>
-      <c r="B983" s="10"/>
-      <c r="C983" s="8"/>
-      <c r="D983" s="10"/>
-      <c r="E983" s="10"/>
-      <c r="F983" s="10"/>
-      <c r="G983" s="10"/>
+    <row r="983" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H983" s="1"/>
       <c r="I983" s="1"/>
       <c r="J983" s="1"/>
@@ -29369,14 +28737,7 @@
       <c r="Y983" s="1"/>
       <c r="Z983" s="1"/>
     </row>
-    <row r="984" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A984" s="10"/>
-      <c r="B984" s="10"/>
-      <c r="C984" s="8"/>
-      <c r="D984" s="10"/>
-      <c r="E984" s="10"/>
-      <c r="F984" s="10"/>
-      <c r="G984" s="10"/>
+    <row r="984" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H984" s="1"/>
       <c r="I984" s="1"/>
       <c r="J984" s="1"/>
@@ -29397,14 +28758,7 @@
       <c r="Y984" s="1"/>
       <c r="Z984" s="1"/>
     </row>
-    <row r="985" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A985" s="10"/>
-      <c r="B985" s="10"/>
-      <c r="C985" s="8"/>
-      <c r="D985" s="10"/>
-      <c r="E985" s="10"/>
-      <c r="F985" s="10"/>
-      <c r="G985" s="10"/>
+    <row r="985" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H985" s="1"/>
       <c r="I985" s="1"/>
       <c r="J985" s="1"/>
@@ -29425,14 +28779,7 @@
       <c r="Y985" s="1"/>
       <c r="Z985" s="1"/>
     </row>
-    <row r="986" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A986" s="10"/>
-      <c r="B986" s="10"/>
-      <c r="C986" s="8"/>
-      <c r="D986" s="10"/>
-      <c r="E986" s="10"/>
-      <c r="F986" s="10"/>
-      <c r="G986" s="10"/>
+    <row r="986" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H986" s="1"/>
       <c r="I986" s="1"/>
       <c r="J986" s="1"/>
@@ -29453,14 +28800,7 @@
       <c r="Y986" s="1"/>
       <c r="Z986" s="1"/>
     </row>
-    <row r="987" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A987" s="10"/>
-      <c r="B987" s="10"/>
-      <c r="C987" s="8"/>
-      <c r="D987" s="10"/>
-      <c r="E987" s="10"/>
-      <c r="F987" s="10"/>
-      <c r="G987" s="10"/>
+    <row r="987" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H987" s="1"/>
       <c r="I987" s="1"/>
       <c r="J987" s="1"/>
@@ -29481,14 +28821,7 @@
       <c r="Y987" s="1"/>
       <c r="Z987" s="1"/>
     </row>
-    <row r="988" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A988" s="10"/>
-      <c r="B988" s="10"/>
-      <c r="C988" s="8"/>
-      <c r="D988" s="10"/>
-      <c r="E988" s="10"/>
-      <c r="F988" s="10"/>
-      <c r="G988" s="10"/>
+    <row r="988" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H988" s="1"/>
       <c r="I988" s="1"/>
       <c r="J988" s="1"/>
@@ -29509,14 +28842,7 @@
       <c r="Y988" s="1"/>
       <c r="Z988" s="1"/>
     </row>
-    <row r="989" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A989" s="10"/>
-      <c r="B989" s="10"/>
-      <c r="C989" s="8"/>
-      <c r="D989" s="10"/>
-      <c r="E989" s="10"/>
-      <c r="F989" s="10"/>
-      <c r="G989" s="10"/>
+    <row r="989" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H989" s="1"/>
       <c r="I989" s="1"/>
       <c r="J989" s="1"/>
@@ -29537,14 +28863,7 @@
       <c r="Y989" s="1"/>
       <c r="Z989" s="1"/>
     </row>
-    <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A990" s="10"/>
-      <c r="B990" s="10"/>
-      <c r="C990" s="8"/>
-      <c r="D990" s="10"/>
-      <c r="E990" s="10"/>
-      <c r="F990" s="10"/>
-      <c r="G990" s="10"/>
+    <row r="990" spans="8:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H990" s="1"/>
       <c r="I990" s="1"/>
       <c r="J990" s="1"/>

</xml_diff>